<commit_message>
Updated dev and production testing log. Add Trello screenshot
</commit_message>
<xml_diff>
--- a/docs/testing/User_testing_log_internal.xlsx
+++ b/docs/testing/User_testing_log_internal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kathe/academy/assignments/Term 3/T3A2_1UpBouldering/t3a2-full-stack-app-docs/docs/testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10B3337-2C4D-4E4F-AC98-503F5DBD174B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A1C9C8-1775-8C40-9D8B-8E9B3BA20516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="500" windowWidth="28720" windowHeight="17500" xr2:uid="{D817E636-62B6-FF4B-A827-BB0242BF58CC}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Test_site_functionality" sheetId="1" r:id="rId1"/>
     <sheet name="Test_site_layout" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="57">
   <si>
     <t>Page</t>
   </si>
@@ -169,6 +169,109 @@
 Tablet
 Desktop</t>
     </r>
+  </si>
+  <si>
+    <t>Process</t>
+  </si>
+  <si>
+    <t>User sign up process</t>
+  </si>
+  <si>
+    <t>Check In page</t>
+  </si>
+  <si>
+    <t>Log In page</t>
+  </si>
+  <si>
+    <t>Sign Up page</t>
+  </si>
+  <si>
+    <t>Page should render check-in instructions and email field</t>
+  </si>
+  <si>
+    <t>OK - no issues</t>
+  </si>
+  <si>
+    <t>Page should render log-in instructions, email field, password field and link for password reset</t>
+  </si>
+  <si>
+    <t>Forgot password page</t>
+  </si>
+  <si>
+    <t>Page should render password reset instructions and email field</t>
+  </si>
+  <si>
+    <t>OK - no issues
+Process is intuitive and straightforward</t>
+  </si>
+  <si>
+    <t>User details page</t>
+  </si>
+  <si>
+    <t>Photo upload</t>
+  </si>
+  <si>
+    <t>Open dialogue box to upload user image
+Image should preview should display</t>
+  </si>
+  <si>
+    <t>Drag and drop to upload user image
+Image should preview should display</t>
+  </si>
+  <si>
+    <t>OK - no issues
+Image preview displays correctly</t>
+  </si>
+  <si>
+    <t>Page should collect user sign up information and profile image</t>
+  </si>
+  <si>
+    <t>Waiver</t>
+  </si>
+  <si>
+    <t>Signature process</t>
+  </si>
+  <si>
+    <t>Waiver should display and prompt user for signature</t>
+  </si>
+  <si>
+    <t>Signature box should appear for user to sign with mouse</t>
+  </si>
+  <si>
+    <t>OK - Waiver displays correctly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK - Signature field appears and process works as expected. Reset also works. </t>
+  </si>
+  <si>
+    <t>Payment page</t>
+  </si>
+  <si>
+    <t>Monthly or annual subscription options should display</t>
+  </si>
+  <si>
+    <t>Page should prompt for user email, password, password confirmation</t>
+  </si>
+  <si>
+    <t>Date of test - Development</t>
+  </si>
+  <si>
+    <t>Date of test - Production</t>
+  </si>
+  <si>
+    <t>Favicon appears correctly but is difficult to see against the grey background. Suggest we add a black background for contrast</t>
+  </si>
+  <si>
+    <t>Ongoing</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>N/A - home page was temporary placeholder and has not been replaced</t>
+  </si>
+  <si>
+    <t>Process should follow the logic of the site map and wireframe prototypes</t>
   </si>
 </sst>
 </file>
@@ -246,7 +349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -293,8 +396,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="15" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -610,124 +728,146 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE7D472-0340-AA48-BD2C-6CD5BBBBE0B5}">
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:R28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.1640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="15"/>
-    <col min="4" max="4" width="16.33203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="49.6640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.5" style="12" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="15"/>
+    <col min="3" max="3" width="20.1640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" style="19" customWidth="1"/>
+    <col min="6" max="6" width="38.5" style="14" customWidth="1"/>
     <col min="7" max="7" width="18.1640625" style="12" customWidth="1"/>
-    <col min="8" max="8" width="20.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.1640625" style="13" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="3"/>
+    <col min="8" max="8" width="16.1640625" style="21" customWidth="1"/>
+    <col min="9" max="9" width="30.33203125" style="17" customWidth="1"/>
+    <col min="10" max="10" width="15.1640625" style="13" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1" ht="100" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="2" customFormat="1" ht="100" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>2</v>
+      <c r="B1" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="E1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="M1" s="1"/>
+      <c r="K1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R1" s="1"/>
+    </row>
+    <row r="2" spans="1:18" ht="100" x14ac:dyDescent="0.2">
       <c r="A2" s="15">
         <v>1</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="18">
         <v>44396</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="14" t="s">
         <v>18</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="H2" s="20">
+        <v>44398</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="20" x14ac:dyDescent="0.2">
       <c r="A3" s="15">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="18">
         <v>44396</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="14" t="s">
         <v>17</v>
       </c>
       <c r="G3" s="12" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" ht="80" x14ac:dyDescent="0.2">
+      <c r="H3" s="20">
+        <v>44398</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="80" x14ac:dyDescent="0.2">
       <c r="A4" s="15">
-        <f t="shared" ref="A4:A25" si="0">A3+1</f>
+        <f t="shared" ref="A4:A28" si="0">A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="18">
         <v>44396</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>13</v>
       </c>
       <c r="F4" s="14" t="s">
         <v>14</v>
@@ -735,75 +875,381 @@
       <c r="G4" s="12" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="H4" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="40" x14ac:dyDescent="0.2">
       <c r="A5" s="15">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="N5" s="1"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B5" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="18">
+        <v>44398</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="20">
+        <v>44398</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="1:18" ht="40" x14ac:dyDescent="0.2">
       <c r="A6" s="15">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B6" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="18">
+        <v>44398</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="20">
+        <v>44398</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="40" x14ac:dyDescent="0.2">
       <c r="A7" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B7" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="18">
+        <v>44398</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="20">
+        <v>44398</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="40" x14ac:dyDescent="0.2">
       <c r="A8" s="15">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B8" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="18">
+        <v>44398</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="20">
+        <v>44398</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="40" x14ac:dyDescent="0.2">
       <c r="A9" s="15">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B9" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="18">
+        <v>44398</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="20">
+        <v>44398</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="40" x14ac:dyDescent="0.2">
       <c r="A10" s="15">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B10" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="18">
+        <v>44398</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="20">
+        <v>44398</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="40" x14ac:dyDescent="0.2">
       <c r="A11" s="15">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B11" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="18">
+        <v>44398</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="20">
+        <v>44398</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="40" x14ac:dyDescent="0.2">
       <c r="A12" s="15">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B12" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="18">
+        <v>44398</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="20">
+        <v>44398</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="60" x14ac:dyDescent="0.2">
       <c r="A13" s="15">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B13" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="18">
+        <v>44398</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="20">
+        <v>44398</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="40" x14ac:dyDescent="0.2">
       <c r="A14" s="15">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B14" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="18">
+        <v>44398</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="20">
+        <v>44398</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="40" x14ac:dyDescent="0.2">
       <c r="A15" s="15">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B15" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="18">
+        <v>44398</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="20">
+        <v>44398</v>
+      </c>
+      <c r="I15" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="15">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -865,8 +1311,20 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="15">
-        <f>A25+1</f>
+        <f t="shared" si="0"/>
         <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="15">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="15">
+        <f t="shared" si="0"/>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add client prototype survey raw data and description in ReadMe. Add trello screenshot. Updates to internal user testing log
</commit_message>
<xml_diff>
--- a/docs/testing/User_testing_log_internal.xlsx
+++ b/docs/testing/User_testing_log_internal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kathe/academy/assignments/Term 3/T3A2_1UpBouldering/t3a2-full-stack-app-docs/docs/testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A1C9C8-1775-8C40-9D8B-8E9B3BA20516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC2C2DC7-ECFE-D54F-85AB-A0D77ED31121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="500" windowWidth="28720" windowHeight="17500" xr2:uid="{D817E636-62B6-FF4B-A827-BB0242BF58CC}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="59">
   <si>
     <t>Page</t>
   </si>
@@ -272,6 +272,12 @@
   </si>
   <si>
     <t>Process should follow the logic of the site map and wireframe prototypes</t>
+  </si>
+  <si>
+    <t>Password reset</t>
+  </si>
+  <si>
+    <t>Submitting email should send password reset instructions</t>
   </si>
 </sst>
 </file>
@@ -731,7 +737,8 @@
   <dimension ref="A1:R28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -787,7 +794,7 @@
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
     </row>
-    <row r="2" spans="1:18" ht="100" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="88" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15">
         <v>1</v>
       </c>
@@ -1249,11 +1256,30 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" ht="40" x14ac:dyDescent="0.2">
       <c r="A16" s="15">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
+      <c r="B16" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="18">
+        <v>44401</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="20"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="15">

</xml_diff>